<commit_message>
fixed reports and updated scripts
</commit_message>
<xml_diff>
--- a/Reports/Maddy/Repairs_Report.xlsx
+++ b/Reports/Maddy/Repairs_Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitHub\CIS3365\Reports\Maddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15808B37-43AD-4129-8346-C1931CDD6AA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A88F2E1-96D7-442F-BBFE-18A09A7C0A4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DF3CEA9A-8C14-4D15-B067-CBE4CA49C96A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E546E05-1C70-4BA8-830F-97967ADF3A5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>REPAIRS</t>
   </si>
   <si>
-    <t>TRAILER REPAIRS</t>
+    <t>HOOD REPAIR</t>
+  </si>
+  <si>
+    <t>REPAIR BED FLOOR</t>
+  </si>
+  <si>
+    <t>REPAIR TRAILER</t>
+  </si>
+  <si>
+    <t>REPAIR DUMP BOX</t>
   </si>
   <si>
     <t>Service ID</t>
@@ -51,8 +60,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -95,9 +112,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,29 +429,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB8CA2B-7DEF-41A6-A179-776A7C3F6B20}">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E937177-16CF-4684-9B64-465CBE58F84D}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -441,7 +459,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -449,74 +467,26 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>35</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>91</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>92</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>94</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>96</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>98</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>